<commit_message>
Added TestTest to Protein Intake
</commit_message>
<xml_diff>
--- a/Protein_Intake.xlsx
+++ b/Protein_Intake.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\D\archiv\dokumente\privat\Rezepte\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\D\archiv\dokumente\TrainingPlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9BC04F-6206-4B06-B612-957B60D51B78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22ABFFA2-481B-4037-AA14-6535040650FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Breakfast</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Ready-Made Bami Goreng</t>
+  </si>
+  <si>
+    <t>TestTest</t>
   </si>
 </sst>
 </file>
@@ -493,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,6 +843,11 @@
         <v>43.421052631578952</v>
       </c>
     </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>